<commit_message>
added comments to the ResourcesPageTest
</commit_message>
<xml_diff>
--- a/resources/TestData.xlsx
+++ b/resources/TestData.xlsx
@@ -14,17 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Test Case Name</t>
   </si>
   <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>NewResourceTitle</t>
   </si>
   <si>
@@ -37,110 +31,86 @@
     <t>PlaceToSave</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>newResource</t>
+  </si>
+  <si>
+    <t>newResource</t>
+  </si>
+  <si>
+    <t>newResource</t>
+  </si>
+  <si>
+    <t>В розділі "Ресурси"</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>newResource1</t>
+  </si>
+  <si>
+    <t>newResource1</t>
+  </si>
+  <si>
+    <t>newResource1</t>
+  </si>
+  <si>
+    <t>У верхньому меню</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>newResource2</t>
+  </si>
+  <si>
+    <t>newResource2</t>
+  </si>
+  <si>
+    <t>newResource2</t>
+  </si>
+  <si>
+    <t>В розділі "Ресурси"</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>newResource4</t>
+  </si>
+  <si>
+    <t>newResource4</t>
+  </si>
+  <si>
+    <t>newResource4</t>
+  </si>
+  <si>
+    <t>У верхньому меню</t>
+  </si>
+  <si>
     <t>TextToAdd</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>admin@.com</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>newResource</t>
-  </si>
-  <si>
-    <t>newResource</t>
-  </si>
-  <si>
-    <t>newResource</t>
-  </si>
-  <si>
-    <t>В розділі "Ресурси"</t>
-  </si>
-  <si>
-    <t>aaaatttt</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>admin@.com</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>newResource1</t>
-  </si>
-  <si>
-    <t>newResource1</t>
-  </si>
-  <si>
-    <t>newResource1</t>
-  </si>
-  <si>
-    <t>У верхньому меню</t>
-  </si>
-  <si>
-    <t>zzzzz</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>admin@.com</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>newResource2</t>
-  </si>
-  <si>
-    <t>newResource2</t>
-  </si>
-  <si>
-    <t>newResource2</t>
-  </si>
-  <si>
-    <t>В розділі "Ресурси"</t>
-  </si>
-  <si>
-    <t>bug</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>admin@.com</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>newResource4</t>
-  </si>
-  <si>
-    <t>newResource4</t>
-  </si>
-  <si>
-    <t>newResource4</t>
-  </si>
-  <si>
-    <t>У верхньому меню</t>
-  </si>
-  <si>
-    <t>bhbbh</t>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>fdg</t>
+  </si>
+  <si>
+    <t>bggj</t>
+  </si>
+  <si>
+    <t>avffd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -148,12 +118,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -188,7 +152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,24 +454,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,127 +487,90 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="F3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
+    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>